<commit_message>
Add dynamic selector for "Posteaza"
</commit_message>
<xml_diff>
--- a/Grandma-Bot/Mesaje.xlsx
+++ b/Grandma-Bot/Mesaje.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STF-PC\Documents\GitHub\UiPath\OpenGoogleAndSearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STF-PC\Documents\GitHub\UiPath\Grandma-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CFED4-9F29-4079-983D-7287397279E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24C5967-1B79-49A7-AF21-9EDD65121082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Hai trezeste-te odata, cafeluta te asteapta, ca sa-ti faca ziua buna, toate sa iti mearga struna!</t>
   </si>
   <si>
-    <t>Buna dimineata! Cafelua e servita, va astept cu drag!</t>
-  </si>
-  <si>
     <t>O noua zi, un nou inceput… Sa fim sanatosi cu totii si sa ne mearga totul bine!</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>Buna dimineata! Spune, orice-ar fi, buna dimineata, fiindca-n zori de zi reincepe viata!</t>
+  </si>
+  <si>
+    <t>Buna dimineata! Cafeluta e servita, va astept cu drag!</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:A76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,37 +413,37 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>